<commit_message>
+ update http & sql
</commit_message>
<xml_diff>
--- a/test-output/test-name_Regression_Test.xlsx
+++ b/test-output/test-name_Regression_Test.xlsx
@@ -13,12 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Report Time</t>
   </si>
   <si>
-    <t>2022-06-07T09:59:32.753964600</t>
+    <t>2022-06-07T18:01:30.988113500</t>
   </si>
   <si>
     <t>Suite Name</t>
@@ -57,10 +57,10 @@
     <t>Nạp tiền thành công</t>
   </si>
   <si>
-    <t>PASSED</t>
-  </si>
-  <si>
-    <t>00:00:16.664</t>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>00:00:59.768</t>
   </si>
   <si>
     <t>go to detail</t>
@@ -91,6 +91,70 @@
   </si>
   <si>
     <t>Giao dịch thành công</t>
+  </si>
+  <si>
+    <t xml:space="preserve">java.lang.Exception: False to find 'Xác nhận/Text'!
+	at helper.ElementHelper.findElementByAccessibilityId(ElementHelper.java:77)
+	at reader.CashinReader.read(CashinReader.java:53)
+	at reader.CashinReader.read(CashinReader.java:8)
+	at com.automation.test.reader.AbstractReader.getData(AbstractReader.java:15)
+	at com.automation.test.TestVerification.getActual(TestVerification.java:85)
+	at com.automation.test.TestVerification.isOk(TestVerification.java:122)
+	at com.automation.test.TestAction.run(TestAction.java:85)
+	at com.automation.test.TestCase.run(TestCase.java:43)
+	at FirstAndroidTest.enterForm(FirstAndroidTest.java:53)
+	at java.base/jdk.internal.reflect.DirectMethodHandleAccessor.invoke(DirectMethodHandleAccessor.java:104)
+	at java.base/java.lang.reflect.Method.invoke(Method.java:577)
+	at org.testng.internal.invokers.MethodInvocationHelper.invokeMethod(MethodInvocationHelper.java:139)
+	at org.testng.internal.invokers.TestInvoker.invokeMethod(TestInvoker.java:677)
+	at org.testng.internal.invokers.TestInvoker.invokeTestMethod(TestInvoker.java:221)
+	at org.testng.internal.invokers.MethodRunner.runInSequence(MethodRunner.java:50)
+	at org.testng.internal.invokers.TestInvoker$MethodInvocationAgent.invoke(TestInvoker.java:962)
+	at org.testng.internal.invokers.TestInvoker.invokeTestMethods(TestInvoker.java:194)
+	at org.testng.internal.invokers.TestMethodWorker.invokeTestMethods(TestMethodWorker.java:148)
+	at org.testng.internal.invokers.TestMethodWorker.run(TestMethodWorker.java:128)
+	at java.base/java.util.ArrayList.forEach(ArrayList.java:1511)
+	at org.testng.TestRunner.privateRun(TestRunner.java:806)
+	at org.testng.TestRunner.run(TestRunner.java:601)
+	at org.testng.SuiteRunner.runTest(SuiteRunner.java:433)
+	at org.testng.SuiteRunner.runSequentially(SuiteRunner.java:427)
+	at org.testng.SuiteRunner.privateRun(SuiteRunner.java:387)
+	at org.testng.SuiteRunner.run(SuiteRunner.java:330)
+	at org.testng.SuiteRunnerWorker.runSuite(SuiteRunnerWorker.java:52)
+	at org.testng.SuiteRunnerWorker.run(SuiteRunnerWorker.java:95)
+	at org.testng.TestNG.runSuitesSequentially(TestNG.java:1256)
+	at org.testng.TestNG.runSuitesLocally(TestNG.java:1176)
+	at org.testng.TestNG.runSuites(TestNG.java:1099)
+	at org.testng.TestNG.run(TestNG.java:1067)
+	at com.intellij.rt.testng.IDEARemoteTestNG.run(IDEARemoteTestNG.java:66)
+	at com.intellij.rt.testng.RemoteTestNGStarter.main(RemoteTestNGStarter.java:109)
+Caused by: org.openqa.selenium.WebDriverException: An unknown server-side error occurred while processing the command. Original error: 'POST /elements' cannot be proxied to UiAutomator2 server because the instrumentation process is not running (probably crashed). Check the server log and/or the logcat output for more details
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'LONGTRAN2-ITC-C', ip: '10.40.128.103', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '18.0.1.1'
+Driver info: io.appium.java_client.AppiumDriver
+Capabilities {app: D:/JavaCode/app/MOMO.apk, appPackage: vn.momo.platform.test, automationName: Appium, databaseEnabled: false, desired: {app: D:/JavaCode/app/MOMO.apk, automationName: Appium, deviceName: 127.0.0.1:21503, noReset: true, platformName: android, platformVersion: 7.1.2}, deviceApiLevel: 25, deviceManufacturer: google, deviceModel: G011A, deviceName: 127.0.0.1:21503, deviceScreenDensity: 300, deviceScreenSize: 900x1600, deviceUDID: 127.0.0.1:21503, javascriptEnabled: true, locationContextEnabled: false, networkConnectionEnabled: true, noReset: true, pixelRatio: 1.875, platform: LINUX, platformName: Android, platformVersion: 7.1.2, statBarHeight: 45, takesScreenshot: true, viewportRect: {height: 1555, left: 0, top: 45, width: 900}, warnings: {}, webStorageEnabled: false}
+Session ID: 3a10473a-6acf-4958-8705-22c3a629f444
+*** Element info: {Using=accessibility id, value=Xác nhận/Text}
+	at java.base/jdk.internal.reflect.DirectConstructorHandleAccessor.newInstance(DirectConstructorHandleAccessor.java:67)
+	at java.base/java.lang.reflect.Constructor.newInstanceWithCaller(Constructor.java:499)
+	at java.base/java.lang.reflect.Constructor.newInstance(Constructor.java:483)
+	at org.openqa.selenium.remote.http.W3CHttpResponseCodec.createException(W3CHttpResponseCodec.java:187)
+	at org.openqa.selenium.remote.http.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:122)
+	at org.openqa.selenium.remote.http.W3CHttpResponseCodec.decode(W3CHttpResponseCodec.java:49)
+	at org.openqa.selenium.remote.HttpCommandExecutor.execute(HttpCommandExecutor.java:158)
+	at io.appium.java_client.remote.AppiumCommandExecutor.execute(AppiumCommandExecutor.java:250)
+	at org.openqa.selenium.remote.RemoteWebDriver.execute(RemoteWebDriver.java:552)
+	at io.appium.java_client.DefaultGenericMobileDriver.execute(DefaultGenericMobileDriver.java:41)
+	at io.appium.java_client.AppiumDriver.execute(AppiumDriver.java:1)
+	at org.openqa.selenium.remote.RemoteWebDriver.findElements(RemoteWebDriver.java:353)
+	at io.appium.java_client.DefaultGenericMobileDriver.findElements(DefaultGenericMobileDriver.java:53)
+	at io.appium.java_client.AppiumDriver.findElements(AppiumDriver.java:179)
+	at io.appium.java_client.FindsByAccessibilityId.findElementsByAccessibilityId(FindsByAccessibilityId.java:50)
+	at io.appium.java_client.AppiumDriver.findElementsByAccessibilityId(AppiumDriver.java:217)
+	at helper.ElementHelper.findElementByAccessibilityIdIsDisplayed(ElementHelper.java:19)
+	at helper.ElementHelper.findElementByAccessibilityId(ElementHelper.java:73)
+	... 33 more
+</t>
   </si>
 </sst>
 </file>
@@ -287,12 +351,12 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center" horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
       <alignment vertical="center" horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFill="true" applyFont="true" applyBorder="true"/>
@@ -364,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -372,7 +436,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="5">
@@ -409,19 +473,19 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="10" t="n">
         <v>1.0</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>16</v>
       </c>
     </row>
@@ -491,11 +555,11 @@
       <c r="D3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s" s="21">
+      <c r="E3" t="s" s="22">
         <v>14</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>